<commit_message>
fix ccc2/4 and added some cosmetics
</commit_message>
<xml_diff>
--- a/Consolidated Factory Workplan.xlsx
+++ b/Consolidated Factory Workplan.xlsx
@@ -2,21 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Workplans" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="0" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -25,9 +28,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Calibri"/>
       <b val="1"/>
-      <sz val="11"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="18"/>
     </font>
   </fonts>
   <fills count="6">
@@ -39,22 +44,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="00FFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor rgb="00FFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
+        <fgColor rgb="00DDDDDD"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor rgb="00FFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -67,92 +72,68 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right/>
+      <left style="thin"/>
+      <right style="thin"/>
       <top/>
-      <bottom/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -163,24 +144,26 @@
     <xf numFmtId="21" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -543,1137 +526,1109 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B7:K63"/>
+  <dimension ref="B3:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="17.28515625" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="10" bestFit="1" customWidth="1" min="3" max="3"/>
-    <col width="10" bestFit="1" customWidth="1" min="6" max="6"/>
-    <col width="11.85546875" bestFit="1" customWidth="1" min="10" max="10"/>
-  </cols>
   <sheetData>
+    <row r="3">
+      <c r="B3" s="1" t="inlineStr">
+        <is>
+          <t>Consolidated Factory Workplan</t>
+        </is>
+      </c>
+    </row>
+    <row r="4"/>
+    <row r="5">
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Updated on :</t>
+        </is>
+      </c>
+      <c r="E5" s="20" t="n">
+        <v>44657.69052837383</v>
+      </c>
+    </row>
     <row r="7">
-      <c r="B7" s="17" t="inlineStr">
+      <c r="B7" s="3" t="inlineStr">
         <is>
           <t>Factory/Site</t>
         </is>
       </c>
-      <c r="C7" s="12" t="n"/>
-      <c r="D7" s="17" t="inlineStr">
+      <c r="C7" s="4" t="n"/>
+      <c r="D7" s="3" t="inlineStr">
         <is>
           <t>CCC4</t>
         </is>
       </c>
-      <c r="E7" s="12" t="n"/>
-      <c r="F7" s="17" t="inlineStr">
+      <c r="E7" s="4" t="n"/>
+      <c r="F7" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G7" s="12" t="n"/>
-      <c r="H7" s="17" t="inlineStr">
-        <is>
-          <t>Mar-11</t>
-        </is>
-      </c>
-      <c r="J7" s="11" t="inlineStr">
+      <c r="G7" s="4" t="n"/>
+      <c r="H7" s="3" t="inlineStr">
+        <is>
+          <t>Mar.10</t>
+        </is>
+      </c>
+      <c r="J7" s="5" t="inlineStr">
         <is>
           <t>Legend</t>
         </is>
       </c>
-      <c r="K7" s="12" t="n"/>
+      <c r="K7" s="4" t="n"/>
     </row>
     <row r="8">
-      <c r="B8" s="2" t="inlineStr">
+      <c r="B8" s="7" t="inlineStr">
         <is>
           <t>Line</t>
         </is>
       </c>
-      <c r="C8" s="3" t="inlineStr">
+      <c r="C8" s="8" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="D8" s="8" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="E8" s="3" t="inlineStr">
+      <c r="E8" s="8" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
-      <c r="F8" s="4" t="inlineStr">
+      <c r="F8" s="9" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="G8" s="4" t="inlineStr">
+      <c r="G8" s="9" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="H8" s="4" t="inlineStr">
+      <c r="H8" s="9" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
-      <c r="J8" s="1" t="inlineStr">
+      <c r="J8" s="6" t="inlineStr">
         <is>
           <t>First shift</t>
         </is>
       </c>
-      <c r="K8" s="5" t="n"/>
+      <c r="K8" s="10" t="n"/>
     </row>
     <row r="9">
-      <c r="B9" s="6" t="inlineStr">
+      <c r="B9" s="11" t="inlineStr">
         <is>
           <t>DT Kitting&amp;Cell</t>
         </is>
       </c>
-      <c r="C9" s="8" t="n">
+      <c r="C9" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D9" s="5" t="n"/>
-      <c r="E9" s="16" t="n">
+      <c r="D9" s="13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E9" s="14" t="n">
         <v>350</v>
       </c>
-      <c r="F9" s="7" t="n"/>
-      <c r="G9" s="7" t="n"/>
-      <c r="H9" s="7" t="n"/>
-      <c r="J9" s="1" t="inlineStr">
+      <c r="F9" s="12" t="n"/>
+      <c r="G9" s="12" t="n"/>
+      <c r="H9" s="12" t="n"/>
+      <c r="J9" s="6" t="inlineStr">
         <is>
           <t>Second shift</t>
         </is>
       </c>
-      <c r="K9" s="7" t="n"/>
+      <c r="K9" s="12" t="n"/>
     </row>
     <row r="10">
-      <c r="B10" s="6" t="inlineStr">
+      <c r="B10" s="11" t="inlineStr">
         <is>
           <t>DT Backend</t>
         </is>
       </c>
-      <c r="C10" s="8" t="n">
+      <c r="C10" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D10" s="5" t="n"/>
+      <c r="D10" s="13" t="n">
+        <v>0.875</v>
+      </c>
       <c r="E10" s="15" t="n"/>
-      <c r="F10" s="7" t="n"/>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="n"/>
+      <c r="F10" s="12" t="n"/>
+      <c r="G10" s="12" t="n"/>
+      <c r="H10" s="12" t="n"/>
     </row>
     <row r="11">
-      <c r="B11" s="6" t="inlineStr">
+      <c r="B11" s="11" t="inlineStr">
         <is>
           <t>SV Kitting&amp;Cell K6</t>
         </is>
       </c>
-      <c r="C11" s="8" t="n">
+      <c r="C11" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D11" s="5" t="n"/>
-      <c r="E11" s="16" t="n">
+      <c r="D11" s="13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E11" s="14" t="n">
         <v>50</v>
       </c>
-      <c r="F11" s="9" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="G11" s="7" t="n"/>
-      <c r="H11" s="13" t="n">
+      <c r="F11" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G11" s="17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H11" s="18" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="6" t="inlineStr">
+      <c r="B12" s="11" t="inlineStr">
         <is>
           <t>SV Kitting&amp;Cell K7</t>
         </is>
       </c>
-      <c r="C12" s="8" t="n">
+      <c r="C12" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D12" s="5" t="n"/>
-      <c r="E12" s="14" t="n"/>
-      <c r="F12" s="9" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="14" t="n"/>
+      <c r="D12" s="13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E12" s="16" t="n"/>
+      <c r="F12" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G12" s="17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H12" s="16" t="n"/>
     </row>
     <row r="13">
-      <c r="B13" s="6" t="inlineStr">
+      <c r="B13" s="11" t="inlineStr">
         <is>
           <t>SV Backend</t>
         </is>
       </c>
-      <c r="C13" s="8" t="n">
+      <c r="C13" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D13" s="5" t="n"/>
+      <c r="D13" s="13" t="n">
+        <v>0.875</v>
+      </c>
       <c r="E13" s="15" t="n"/>
-      <c r="F13" s="9" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="G13" s="7" t="n"/>
+      <c r="F13" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G13" s="17" t="n">
+        <v>0.25</v>
+      </c>
       <c r="H13" s="15" t="n"/>
     </row>
     <row r="14">
-      <c r="B14" s="6" t="inlineStr">
+      <c r="B14" s="11" t="inlineStr">
         <is>
           <t>Storage line</t>
         </is>
       </c>
-      <c r="C14" s="8" t="n">
+      <c r="C14" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="7" t="n"/>
-      <c r="G14" s="7" t="n"/>
-      <c r="H14" s="7" t="n"/>
+      <c r="D14" s="13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E14" s="10" t="n"/>
+      <c r="F14" s="12" t="n"/>
+      <c r="G14" s="12" t="n"/>
+      <c r="H14" s="12" t="n"/>
     </row>
     <row r="15">
-      <c r="B15" s="6" t="inlineStr">
+      <c r="B15" s="11" t="inlineStr">
         <is>
           <t>CFS</t>
         </is>
       </c>
-      <c r="C15" s="8" t="n">
+      <c r="C15" s="13" t="n">
         <v>0.3541666666666667</v>
       </c>
-      <c r="D15" s="5" t="n"/>
-      <c r="E15" s="5" t="n"/>
-      <c r="F15" s="7" t="n"/>
-      <c r="G15" s="7" t="n"/>
-      <c r="H15" s="7" t="n"/>
+      <c r="D15" s="13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E15" s="10" t="n"/>
+      <c r="F15" s="12" t="n"/>
+      <c r="G15" s="12" t="n"/>
+      <c r="H15" s="12" t="n"/>
     </row>
     <row r="16">
-      <c r="B16" s="17" t="inlineStr">
+      <c r="B16" s="3" t="inlineStr">
         <is>
           <t>Factory/Site</t>
         </is>
       </c>
-      <c r="C16" s="12" t="n"/>
-      <c r="D16" s="17" t="inlineStr">
+      <c r="C16" s="4" t="n"/>
+      <c r="D16" s="3" t="inlineStr">
         <is>
           <t>CCC2</t>
         </is>
       </c>
-      <c r="E16" s="12" t="n"/>
-      <c r="F16" s="17" t="inlineStr">
+      <c r="E16" s="4" t="n"/>
+      <c r="F16" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G16" s="12" t="n"/>
-      <c r="H16" s="17" t="inlineStr">
-        <is>
-          <t>Mar-11</t>
+      <c r="G16" s="4" t="n"/>
+      <c r="H16" s="3" t="inlineStr">
+        <is>
+          <t>Mar.10</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="B17" s="2" t="inlineStr">
+      <c r="B17" s="7" t="inlineStr">
         <is>
           <t>Line</t>
         </is>
       </c>
-      <c r="C17" s="3" t="inlineStr">
+      <c r="C17" s="8" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="D17" s="3" t="inlineStr">
+      <c r="D17" s="8" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="E17" s="3" t="inlineStr">
+      <c r="E17" s="8" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
-      <c r="F17" s="4" t="inlineStr">
+      <c r="F17" s="9" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="G17" s="4" t="inlineStr">
+      <c r="G17" s="9" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="H17" s="4" t="inlineStr">
+      <c r="H17" s="9" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="B18" s="6" t="inlineStr">
+      <c r="B18" s="11" t="inlineStr">
         <is>
           <t>DT Kitting&amp;Cell</t>
         </is>
       </c>
-      <c r="C18" s="8" t="n">
+      <c r="C18" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D18" s="5" t="n"/>
-      <c r="E18" s="16" t="n">
+      <c r="D18" s="13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E18" s="14" t="n">
         <v>750</v>
       </c>
-      <c r="F18" s="9" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="G18" s="7" t="n"/>
-      <c r="H18" s="13" t="n">
+      <c r="F18" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G18" s="17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H18" s="18" t="n">
         <v>700</v>
       </c>
     </row>
     <row r="19">
-      <c r="B19" s="6" t="inlineStr">
+      <c r="B19" s="11" t="inlineStr">
         <is>
           <t>DT Backend</t>
         </is>
       </c>
-      <c r="C19" s="8" t="n">
+      <c r="C19" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D19" s="5" t="n"/>
+      <c r="D19" s="13" t="n">
+        <v>0.875</v>
+      </c>
       <c r="E19" s="15" t="n"/>
-      <c r="F19" s="9" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="G19" s="7" t="n"/>
+      <c r="F19" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G19" s="17" t="n">
+        <v>0.25</v>
+      </c>
       <c r="H19" s="15" t="n"/>
     </row>
     <row r="20">
-      <c r="B20" s="6" t="inlineStr">
+      <c r="B20" s="11" t="inlineStr">
         <is>
           <t>SV Kitting&amp;Cell</t>
         </is>
       </c>
-      <c r="C20" s="8" t="n">
+      <c r="C20" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D20" s="5" t="n"/>
-      <c r="E20" s="16" t="n">
+      <c r="D20" s="13" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="E20" s="14" t="n">
         <v>120</v>
       </c>
-      <c r="F20" s="9" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="G20" s="7" t="n"/>
-      <c r="H20" s="13" t="n">
+      <c r="F20" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G20" s="17" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H20" s="18" t="n">
         <v>100</v>
       </c>
     </row>
     <row r="21">
-      <c r="B21" s="6" t="inlineStr">
+      <c r="B21" s="11" t="inlineStr">
         <is>
           <t>SV Backend</t>
         </is>
       </c>
-      <c r="C21" s="8" t="n">
+      <c r="C21" s="13" t="n">
         <v>0.5138888888888888</v>
       </c>
-      <c r="D21" s="5" t="n"/>
+      <c r="D21" s="13" t="n">
+        <v>0.875</v>
+      </c>
       <c r="E21" s="15" t="n"/>
-      <c r="F21" s="9" t="n">
-        <v>0.875</v>
-      </c>
-      <c r="G21" s="7" t="n"/>
+      <c r="F21" s="17" t="n">
+        <v>0.875</v>
+      </c>
+      <c r="G21" s="17" t="n">
+        <v>0.25</v>
+      </c>
       <c r="H21" s="15" t="n"/>
     </row>
     <row r="22">
-      <c r="B22" s="6" t="inlineStr">
+      <c r="B22" s="11" t="inlineStr">
         <is>
           <t>K8 line</t>
         </is>
       </c>
-      <c r="C22" s="8" t="n">
+      <c r="C22" s="19" t="inlineStr"/>
+      <c r="D22" s="19" t="inlineStr"/>
+      <c r="E22" s="10" t="n"/>
+      <c r="F22" s="12" t="n"/>
+      <c r="G22" s="17" t="n">
         <v>0.3541666666666667</v>
       </c>
-      <c r="D22" s="5" t="n"/>
-      <c r="E22" s="5" t="n"/>
-      <c r="F22" s="7" t="n"/>
-      <c r="G22" s="7" t="n"/>
-      <c r="H22" s="7" t="n"/>
+      <c r="H22" s="12" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="6" t="inlineStr">
+      <c r="B23" s="11" t="inlineStr">
         <is>
           <t>ARB</t>
         </is>
       </c>
-      <c r="C23" s="8" t="n">
+      <c r="C23" s="13" t="n">
         <v>0.3541666666666667</v>
       </c>
-      <c r="D23" s="5" t="n"/>
-      <c r="E23" s="5" t="n"/>
-      <c r="F23" s="7" t="n"/>
-      <c r="G23" s="7" t="n"/>
-      <c r="H23" s="7" t="n"/>
+      <c r="D23" s="13" t="n">
+        <v>0.7291666666666666</v>
+      </c>
+      <c r="E23" s="10" t="n"/>
+      <c r="F23" s="12" t="n"/>
+      <c r="G23" s="12" t="n"/>
+      <c r="H23" s="12" t="n"/>
     </row>
     <row r="24">
-      <c r="B24" s="17" t="inlineStr">
+      <c r="B24" s="3" t="inlineStr">
         <is>
           <t>Factory/Site</t>
         </is>
       </c>
-      <c r="C24" s="12" t="n"/>
-      <c r="D24" s="17" t="inlineStr">
+      <c r="C24" s="4" t="n"/>
+      <c r="D24" s="3" t="inlineStr">
         <is>
           <t>CCC6</t>
         </is>
       </c>
-      <c r="E24" s="12" t="n"/>
-      <c r="F24" s="17" t="inlineStr">
+      <c r="E24" s="4" t="n"/>
+      <c r="F24" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G24" s="12" t="n"/>
-      <c r="H24" s="17" t="n"/>
+      <c r="G24" s="4" t="n"/>
+      <c r="H24" s="3" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="B25" s="2" t="inlineStr">
+      <c r="B25" s="7" t="inlineStr">
         <is>
           <t>Line</t>
         </is>
       </c>
-      <c r="C25" s="3" t="inlineStr">
+      <c r="C25" s="8" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="D25" s="3" t="inlineStr">
+      <c r="D25" s="8" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="E25" s="3" t="inlineStr">
+      <c r="E25" s="8" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
-      <c r="F25" s="4" t="inlineStr">
+      <c r="F25" s="9" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="G25" s="4" t="inlineStr">
+      <c r="G25" s="9" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="H25" s="4" t="inlineStr">
+      <c r="H25" s="9" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
     </row>
     <row r="26">
-      <c r="B26" s="6" t="n"/>
-      <c r="C26" s="5" t="n"/>
-      <c r="D26" s="5" t="n"/>
-      <c r="E26" s="5" t="n"/>
-      <c r="F26" s="7" t="n"/>
-      <c r="G26" s="7" t="n"/>
-      <c r="H26" s="7" t="n"/>
+      <c r="B26" s="11" t="n"/>
+      <c r="C26" s="10" t="n"/>
+      <c r="D26" s="10" t="n"/>
+      <c r="E26" s="10" t="n"/>
+      <c r="F26" s="12" t="n"/>
+      <c r="G26" s="12" t="n"/>
+      <c r="H26" s="12" t="n"/>
     </row>
     <row r="27">
-      <c r="B27" s="6" t="n"/>
-      <c r="C27" s="5" t="n"/>
-      <c r="D27" s="5" t="n"/>
-      <c r="E27" s="5" t="n"/>
-      <c r="F27" s="7" t="n"/>
-      <c r="G27" s="7" t="n"/>
-      <c r="H27" s="7" t="n"/>
+      <c r="B27" s="11" t="n"/>
+      <c r="C27" s="10" t="n"/>
+      <c r="D27" s="10" t="n"/>
+      <c r="E27" s="10" t="n"/>
+      <c r="F27" s="12" t="n"/>
+      <c r="G27" s="12" t="n"/>
+      <c r="H27" s="12" t="n"/>
     </row>
     <row r="28">
-      <c r="B28" s="6" t="n"/>
-      <c r="C28" s="5" t="n"/>
-      <c r="D28" s="5" t="n"/>
-      <c r="E28" s="5" t="n"/>
-      <c r="F28" s="7" t="n"/>
-      <c r="G28" s="7" t="n"/>
-      <c r="H28" s="7" t="n"/>
+      <c r="B28" s="11" t="n"/>
+      <c r="C28" s="10" t="n"/>
+      <c r="D28" s="10" t="n"/>
+      <c r="E28" s="10" t="n"/>
+      <c r="F28" s="12" t="n"/>
+      <c r="G28" s="12" t="n"/>
+      <c r="H28" s="12" t="n"/>
     </row>
     <row r="29">
-      <c r="B29" s="6" t="n"/>
-      <c r="C29" s="5" t="n"/>
-      <c r="D29" s="5" t="n"/>
-      <c r="E29" s="5" t="n"/>
-      <c r="F29" s="7" t="n"/>
-      <c r="G29" s="7" t="n"/>
-      <c r="H29" s="7" t="n"/>
+      <c r="B29" s="11" t="n"/>
+      <c r="C29" s="10" t="n"/>
+      <c r="D29" s="10" t="n"/>
+      <c r="E29" s="10" t="n"/>
+      <c r="F29" s="12" t="n"/>
+      <c r="G29" s="12" t="n"/>
+      <c r="H29" s="12" t="n"/>
     </row>
     <row r="30">
-      <c r="B30" s="6" t="n"/>
-      <c r="C30" s="5" t="n"/>
-      <c r="D30" s="5" t="n"/>
-      <c r="E30" s="5" t="n"/>
-      <c r="F30" s="7" t="n"/>
-      <c r="G30" s="7" t="n"/>
-      <c r="H30" s="7" t="n"/>
+      <c r="B30" s="11" t="n"/>
+      <c r="C30" s="10" t="n"/>
+      <c r="D30" s="10" t="n"/>
+      <c r="E30" s="10" t="n"/>
+      <c r="F30" s="12" t="n"/>
+      <c r="G30" s="12" t="n"/>
+      <c r="H30" s="12" t="n"/>
     </row>
     <row r="31">
-      <c r="B31" s="6" t="n"/>
-      <c r="C31" s="5" t="n"/>
-      <c r="D31" s="5" t="n"/>
-      <c r="E31" s="5" t="n"/>
-      <c r="F31" s="7" t="n"/>
-      <c r="G31" s="7" t="n"/>
-      <c r="H31" s="7" t="n"/>
+      <c r="B31" s="11" t="n"/>
+      <c r="C31" s="10" t="n"/>
+      <c r="D31" s="10" t="n"/>
+      <c r="E31" s="10" t="n"/>
+      <c r="F31" s="12" t="n"/>
+      <c r="G31" s="12" t="n"/>
+      <c r="H31" s="12" t="n"/>
     </row>
     <row r="32">
-      <c r="B32" s="17" t="inlineStr">
+      <c r="B32" s="3" t="inlineStr">
         <is>
           <t>Factory/Site</t>
         </is>
       </c>
-      <c r="C32" s="12" t="n"/>
-      <c r="D32" s="17" t="inlineStr">
+      <c r="C32" s="4" t="n"/>
+      <c r="D32" s="3" t="inlineStr">
         <is>
           <t>APCC</t>
         </is>
       </c>
-      <c r="E32" s="12" t="n"/>
-      <c r="F32" s="17" t="inlineStr">
+      <c r="E32" s="4" t="n"/>
+      <c r="F32" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G32" s="12" t="n"/>
-      <c r="H32" s="17" t="n"/>
+      <c r="G32" s="4" t="n"/>
+      <c r="H32" s="3" t="inlineStr">
+        <is>
+          <t>22-Feb</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="B33" s="2" t="inlineStr">
+      <c r="B33" s="7" t="inlineStr">
         <is>
           <t>Line</t>
         </is>
       </c>
-      <c r="C33" s="3" t="inlineStr">
+      <c r="C33" s="8" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="D33" s="3" t="inlineStr">
+      <c r="D33" s="8" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="E33" s="3" t="inlineStr">
+      <c r="E33" s="8" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
-      <c r="F33" s="4" t="inlineStr">
+      <c r="F33" s="9" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="G33" s="4" t="inlineStr">
+      <c r="G33" s="9" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="H33" s="4" t="inlineStr">
+      <c r="H33" s="9" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="B34" s="6" t="inlineStr">
+      <c r="B34" s="11" t="inlineStr">
         <is>
           <t>Desktop</t>
         </is>
       </c>
-      <c r="C34" s="5" t="inlineStr">
+      <c r="C34" s="10" t="inlineStr">
         <is>
           <t>8am</t>
         </is>
       </c>
-      <c r="D34" s="5" t="inlineStr">
+      <c r="D34" s="10" t="inlineStr">
         <is>
           <t>7pm</t>
         </is>
       </c>
-      <c r="E34" s="5" t="n"/>
-      <c r="F34" s="7" t="inlineStr">
+      <c r="E34" s="10" t="n"/>
+      <c r="F34" s="12" t="inlineStr">
         <is>
           <t>11am</t>
         </is>
       </c>
-      <c r="G34" s="7" t="inlineStr">
+      <c r="G34" s="12" t="inlineStr">
         <is>
           <t>10pm</t>
         </is>
       </c>
-      <c r="H34" s="7" t="n"/>
+      <c r="H34" s="12" t="n"/>
     </row>
     <row r="35">
-      <c r="B35" s="6" t="inlineStr">
+      <c r="B35" s="11" t="inlineStr">
         <is>
           <t>HYBRID 1</t>
         </is>
       </c>
-      <c r="C35" s="5" t="inlineStr">
+      <c r="C35" s="10" t="inlineStr">
         <is>
           <t>8am</t>
         </is>
       </c>
-      <c r="D35" s="5" t="inlineStr">
+      <c r="D35" s="10" t="inlineStr">
         <is>
           <t>7pm</t>
         </is>
       </c>
-      <c r="E35" s="5" t="n"/>
-      <c r="F35" s="7" t="inlineStr">
+      <c r="E35" s="10" t="n"/>
+      <c r="F35" s="12" t="inlineStr">
         <is>
           <t>11am</t>
         </is>
       </c>
-      <c r="G35" s="7" t="inlineStr">
+      <c r="G35" s="12" t="inlineStr">
         <is>
           <t>10pm</t>
         </is>
       </c>
-      <c r="H35" s="7" t="n"/>
+      <c r="H35" s="12" t="n"/>
     </row>
     <row r="36">
-      <c r="B36" s="6" t="inlineStr">
+      <c r="B36" s="11" t="inlineStr">
         <is>
           <t>HYBRID 2</t>
         </is>
       </c>
-      <c r="C36" s="5" t="inlineStr">
+      <c r="C36" s="10" t="inlineStr">
         <is>
           <t>8am</t>
         </is>
       </c>
-      <c r="D36" s="5" t="inlineStr">
+      <c r="D36" s="10" t="inlineStr">
         <is>
           <t>7pm</t>
         </is>
       </c>
-      <c r="E36" s="5" t="n"/>
-      <c r="F36" s="7" t="inlineStr">
+      <c r="E36" s="10" t="n"/>
+      <c r="F36" s="12" t="inlineStr">
         <is>
           <t>11am</t>
         </is>
       </c>
-      <c r="G36" s="7" t="inlineStr">
+      <c r="G36" s="12" t="inlineStr">
         <is>
           <t>10pm</t>
         </is>
       </c>
-      <c r="H36" s="7" t="n"/>
+      <c r="H36" s="12" t="n"/>
     </row>
     <row r="37">
-      <c r="B37" s="6" t="inlineStr">
+      <c r="B37" s="11" t="inlineStr">
         <is>
           <t>Server</t>
         </is>
       </c>
-      <c r="C37" s="5" t="inlineStr">
+      <c r="C37" s="10" t="inlineStr">
         <is>
           <t>8am</t>
         </is>
       </c>
-      <c r="D37" s="5" t="inlineStr">
+      <c r="D37" s="10" t="inlineStr">
         <is>
           <t>7pm</t>
         </is>
       </c>
-      <c r="E37" s="5" t="n"/>
-      <c r="F37" s="7" t="inlineStr">
+      <c r="E37" s="10" t="n"/>
+      <c r="F37" s="12" t="inlineStr">
         <is>
           <t>11am</t>
         </is>
       </c>
-      <c r="G37" s="7" t="inlineStr">
+      <c r="G37" s="12" t="inlineStr">
         <is>
           <t>10pm</t>
         </is>
       </c>
-      <c r="H37" s="7" t="n"/>
+      <c r="H37" s="12" t="n"/>
     </row>
     <row r="38">
-      <c r="B38" s="6" t="n"/>
-      <c r="C38" s="5" t="n"/>
-      <c r="D38" s="5" t="n"/>
-      <c r="E38" s="5" t="n"/>
-      <c r="F38" s="7" t="n"/>
-      <c r="G38" s="7" t="n"/>
-      <c r="H38" s="7" t="n"/>
+      <c r="B38" s="11" t="n"/>
+      <c r="C38" s="10" t="n"/>
+      <c r="D38" s="10" t="n"/>
+      <c r="E38" s="10" t="n"/>
+      <c r="F38" s="12" t="n"/>
+      <c r="G38" s="12" t="n"/>
+      <c r="H38" s="12" t="n"/>
     </row>
     <row r="39">
-      <c r="B39" s="6" t="n"/>
-      <c r="C39" s="5" t="n"/>
-      <c r="D39" s="5" t="n"/>
-      <c r="E39" s="5" t="n"/>
-      <c r="F39" s="7" t="n"/>
-      <c r="G39" s="7" t="n"/>
-      <c r="H39" s="7" t="n"/>
+      <c r="B39" s="11" t="n"/>
+      <c r="C39" s="10" t="n"/>
+      <c r="D39" s="10" t="n"/>
+      <c r="E39" s="10" t="n"/>
+      <c r="F39" s="12" t="n"/>
+      <c r="G39" s="12" t="n"/>
+      <c r="H39" s="12" t="n"/>
     </row>
     <row r="40">
-      <c r="B40" s="17" t="inlineStr">
+      <c r="B40" s="3" t="inlineStr">
         <is>
           <t>Factory/Site</t>
         </is>
       </c>
-      <c r="C40" s="12" t="n"/>
-      <c r="D40" s="17" t="inlineStr">
+      <c r="C40" s="4" t="n"/>
+      <c r="D40" s="3" t="inlineStr">
         <is>
           <t>ICC</t>
         </is>
       </c>
-      <c r="E40" s="12" t="n"/>
-      <c r="F40" s="17" t="inlineStr">
+      <c r="E40" s="4" t="n"/>
+      <c r="F40" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G40" s="12" t="n"/>
-      <c r="H40" s="17" t="n"/>
+      <c r="G40" s="4" t="n"/>
+      <c r="H40" s="3" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="B41" s="2" t="inlineStr">
+      <c r="B41" s="7" t="inlineStr">
         <is>
           <t>Line</t>
         </is>
       </c>
-      <c r="C41" s="3" t="inlineStr">
+      <c r="C41" s="8" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="D41" s="3" t="inlineStr">
+      <c r="D41" s="8" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="E41" s="3" t="inlineStr">
+      <c r="E41" s="8" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
-      <c r="F41" s="4" t="inlineStr">
+      <c r="F41" s="9" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="G41" s="4" t="inlineStr">
+      <c r="G41" s="9" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="H41" s="4" t="inlineStr">
+      <c r="H41" s="9" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
     </row>
     <row r="42">
-      <c r="B42" s="6" t="inlineStr">
+      <c r="B42" s="11" t="inlineStr">
         <is>
           <t>Line 1 Frontend</t>
         </is>
       </c>
-      <c r="C42" s="5" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="D42" s="5" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="E42" s="5" t="n"/>
-      <c r="F42" s="7" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="G42" s="7" t="inlineStr">
-        <is>
-          <t>23:45</t>
-        </is>
-      </c>
-      <c r="H42" s="7" t="n"/>
+      <c r="C42" s="10" t="n"/>
+      <c r="D42" s="10" t="n"/>
+      <c r="E42" s="10" t="n"/>
+      <c r="F42" s="12" t="n"/>
+      <c r="G42" s="12" t="n"/>
+      <c r="H42" s="12" t="n"/>
     </row>
     <row r="43">
-      <c r="B43" s="6" t="inlineStr">
+      <c r="B43" s="11" t="inlineStr">
         <is>
           <t>Line 2 Frontend</t>
         </is>
       </c>
-      <c r="C43" s="5" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="D43" s="5" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="E43" s="5" t="n"/>
-      <c r="F43" s="7" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="G43" s="7" t="inlineStr">
-        <is>
-          <t>23:45</t>
-        </is>
-      </c>
-      <c r="H43" s="7" t="n"/>
+      <c r="C43" s="10" t="n"/>
+      <c r="D43" s="10" t="n"/>
+      <c r="E43" s="10" t="n"/>
+      <c r="F43" s="12" t="n"/>
+      <c r="G43" s="12" t="n"/>
+      <c r="H43" s="12" t="n"/>
     </row>
     <row r="44">
-      <c r="B44" s="6" t="inlineStr">
+      <c r="B44" s="11" t="inlineStr">
         <is>
           <t>Line 3 Frontend</t>
         </is>
       </c>
-      <c r="C44" s="5" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="D44" s="5" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="E44" s="5" t="n"/>
-      <c r="F44" s="7" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="G44" s="7" t="inlineStr">
-        <is>
-          <t>23:45</t>
-        </is>
-      </c>
-      <c r="H44" s="7" t="n"/>
+      <c r="C44" s="10" t="n"/>
+      <c r="D44" s="10" t="n"/>
+      <c r="E44" s="10" t="n"/>
+      <c r="F44" s="12" t="n"/>
+      <c r="G44" s="12" t="n"/>
+      <c r="H44" s="12" t="n"/>
     </row>
     <row r="45">
-      <c r="B45" s="6" t="inlineStr">
+      <c r="B45" s="11" t="inlineStr">
         <is>
           <t>Line 1 Backend</t>
         </is>
       </c>
-      <c r="C45" s="5" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="D45" s="5" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="E45" s="5" t="n"/>
-      <c r="F45" s="7" t="n"/>
-      <c r="G45" s="7" t="n"/>
-      <c r="H45" s="7" t="n"/>
+      <c r="C45" s="10" t="n"/>
+      <c r="D45" s="10" t="n"/>
+      <c r="E45" s="10" t="n"/>
+      <c r="F45" s="12" t="n"/>
+      <c r="G45" s="12" t="n"/>
+      <c r="H45" s="12" t="n"/>
     </row>
     <row r="46">
-      <c r="B46" s="6" t="inlineStr">
+      <c r="B46" s="11" t="inlineStr">
         <is>
           <t>Line 2 Backend</t>
         </is>
       </c>
-      <c r="C46" s="5" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="D46" s="5" t="inlineStr">
-        <is>
-          <t>23:45</t>
-        </is>
-      </c>
-      <c r="E46" s="5" t="n"/>
-      <c r="F46" s="7" t="n"/>
-      <c r="G46" s="7" t="n"/>
-      <c r="H46" s="7" t="n"/>
+      <c r="C46" s="10" t="n"/>
+      <c r="D46" s="10" t="n"/>
+      <c r="E46" s="10" t="n"/>
+      <c r="F46" s="12" t="n"/>
+      <c r="G46" s="12" t="n"/>
+      <c r="H46" s="12" t="n"/>
     </row>
     <row r="47">
-      <c r="B47" s="6" t="inlineStr">
+      <c r="B47" s="11" t="inlineStr">
         <is>
           <t>Line 3 Backend</t>
         </is>
       </c>
-      <c r="C47" s="5" t="n"/>
-      <c r="D47" s="5" t="n"/>
-      <c r="E47" s="5" t="n"/>
-      <c r="F47" s="7" t="n"/>
-      <c r="G47" s="7" t="n"/>
-      <c r="H47" s="7" t="n"/>
+      <c r="C47" s="10" t="n"/>
+      <c r="D47" s="10" t="n"/>
+      <c r="E47" s="10" t="n"/>
+      <c r="F47" s="12" t="n"/>
+      <c r="G47" s="12" t="n"/>
+      <c r="H47" s="12" t="n"/>
     </row>
     <row r="48">
-      <c r="B48" s="6" t="n"/>
-      <c r="C48" s="5" t="n"/>
-      <c r="D48" s="5" t="n"/>
-      <c r="E48" s="5" t="n"/>
-      <c r="F48" s="7" t="n"/>
-      <c r="G48" s="7" t="n"/>
-      <c r="H48" s="7" t="n"/>
+      <c r="B48" s="11" t="n"/>
+      <c r="C48" s="10" t="n"/>
+      <c r="D48" s="10" t="n"/>
+      <c r="E48" s="10" t="n"/>
+      <c r="F48" s="12" t="n"/>
+      <c r="G48" s="12" t="n"/>
+      <c r="H48" s="12" t="n"/>
     </row>
     <row r="49">
-      <c r="B49" s="17" t="inlineStr">
+      <c r="B49" s="3" t="inlineStr">
         <is>
           <t>Factory/Site</t>
         </is>
       </c>
-      <c r="C49" s="12" t="n"/>
-      <c r="D49" s="17" t="inlineStr">
+      <c r="C49" s="4" t="n"/>
+      <c r="D49" s="3" t="inlineStr">
         <is>
           <t>EMFP</t>
         </is>
       </c>
-      <c r="E49" s="12" t="n"/>
-      <c r="F49" s="17" t="inlineStr">
+      <c r="E49" s="4" t="n"/>
+      <c r="F49" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G49" s="12" t="n"/>
-      <c r="H49" s="17" t="n"/>
+      <c r="G49" s="4" t="n"/>
+      <c r="H49" s="3" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="B50" s="2" t="inlineStr">
+      <c r="B50" s="7" t="inlineStr">
         <is>
           <t>Line</t>
         </is>
       </c>
-      <c r="C50" s="3" t="inlineStr">
+      <c r="C50" s="8" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="D50" s="3" t="inlineStr">
+      <c r="D50" s="8" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="E50" s="3" t="inlineStr">
+      <c r="E50" s="8" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
-      <c r="F50" s="4" t="inlineStr">
+      <c r="F50" s="9" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="G50" s="4" t="inlineStr">
+      <c r="G50" s="9" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="H50" s="4" t="inlineStr">
+      <c r="H50" s="9" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="B51" s="6" t="n"/>
-      <c r="C51" s="5" t="n"/>
-      <c r="D51" s="5" t="n"/>
-      <c r="E51" s="5" t="n"/>
-      <c r="F51" s="7" t="n"/>
-      <c r="G51" s="7" t="n"/>
-      <c r="H51" s="7" t="n"/>
+      <c r="B51" s="11" t="n"/>
+      <c r="C51" s="10" t="n"/>
+      <c r="D51" s="10" t="n"/>
+      <c r="E51" s="10" t="n"/>
+      <c r="F51" s="12" t="n"/>
+      <c r="G51" s="12" t="n"/>
+      <c r="H51" s="12" t="n"/>
     </row>
     <row r="52">
-      <c r="B52" s="6" t="n"/>
-      <c r="C52" s="5" t="n"/>
-      <c r="D52" s="5" t="n"/>
-      <c r="E52" s="5" t="n"/>
-      <c r="F52" s="7" t="n"/>
-      <c r="G52" s="7" t="n"/>
-      <c r="H52" s="7" t="n"/>
+      <c r="B52" s="11" t="n"/>
+      <c r="C52" s="10" t="n"/>
+      <c r="D52" s="10" t="n"/>
+      <c r="E52" s="10" t="n"/>
+      <c r="F52" s="12" t="n"/>
+      <c r="G52" s="12" t="n"/>
+      <c r="H52" s="12" t="n"/>
     </row>
     <row r="53">
-      <c r="B53" s="6" t="n"/>
-      <c r="C53" s="5" t="n"/>
-      <c r="D53" s="5" t="n"/>
-      <c r="E53" s="5" t="n"/>
-      <c r="F53" s="7" t="n"/>
-      <c r="G53" s="7" t="n"/>
-      <c r="H53" s="7" t="n"/>
+      <c r="B53" s="11" t="n"/>
+      <c r="C53" s="10" t="n"/>
+      <c r="D53" s="10" t="n"/>
+      <c r="E53" s="10" t="n"/>
+      <c r="F53" s="12" t="n"/>
+      <c r="G53" s="12" t="n"/>
+      <c r="H53" s="12" t="n"/>
     </row>
     <row r="54">
-      <c r="B54" s="6" t="n"/>
-      <c r="C54" s="5" t="n"/>
-      <c r="D54" s="5" t="n"/>
-      <c r="E54" s="5" t="n"/>
-      <c r="F54" s="7" t="n"/>
-      <c r="G54" s="7" t="n"/>
-      <c r="H54" s="7" t="n"/>
+      <c r="B54" s="11" t="n"/>
+      <c r="C54" s="10" t="n"/>
+      <c r="D54" s="10" t="n"/>
+      <c r="E54" s="10" t="n"/>
+      <c r="F54" s="12" t="n"/>
+      <c r="G54" s="12" t="n"/>
+      <c r="H54" s="12" t="n"/>
     </row>
     <row r="55">
-      <c r="B55" s="6" t="n"/>
-      <c r="C55" s="5" t="n"/>
-      <c r="D55" s="5" t="n"/>
-      <c r="E55" s="5" t="n"/>
-      <c r="F55" s="7" t="n"/>
-      <c r="G55" s="7" t="n"/>
-      <c r="H55" s="7" t="n"/>
+      <c r="B55" s="11" t="n"/>
+      <c r="C55" s="10" t="n"/>
+      <c r="D55" s="10" t="n"/>
+      <c r="E55" s="10" t="n"/>
+      <c r="F55" s="12" t="n"/>
+      <c r="G55" s="12" t="n"/>
+      <c r="H55" s="12" t="n"/>
     </row>
     <row r="56">
-      <c r="B56" s="6" t="n"/>
-      <c r="C56" s="5" t="n"/>
-      <c r="D56" s="5" t="n"/>
-      <c r="E56" s="5" t="n"/>
-      <c r="F56" s="7" t="n"/>
-      <c r="G56" s="7" t="n"/>
-      <c r="H56" s="7" t="n"/>
+      <c r="B56" s="11" t="n"/>
+      <c r="C56" s="10" t="n"/>
+      <c r="D56" s="10" t="n"/>
+      <c r="E56" s="10" t="n"/>
+      <c r="F56" s="12" t="n"/>
+      <c r="G56" s="12" t="n"/>
+      <c r="H56" s="12" t="n"/>
     </row>
     <row r="57">
-      <c r="B57" s="17" t="inlineStr">
+      <c r="B57" s="3" t="inlineStr">
         <is>
           <t>Factory/Site</t>
         </is>
       </c>
-      <c r="C57" s="12" t="n"/>
-      <c r="D57" s="17" t="inlineStr">
+      <c r="C57" s="4" t="n"/>
+      <c r="D57" s="3" t="inlineStr">
         <is>
           <t>BRH1</t>
         </is>
       </c>
-      <c r="E57" s="12" t="n"/>
-      <c r="F57" s="17" t="inlineStr">
+      <c r="E57" s="4" t="n"/>
+      <c r="F57" s="3" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="G57" s="12" t="n"/>
-      <c r="H57" s="17" t="n"/>
+      <c r="G57" s="4" t="n"/>
+      <c r="H57" s="3" t="inlineStr"/>
     </row>
     <row r="58">
-      <c r="B58" s="2" t="inlineStr">
+      <c r="B58" s="7" t="inlineStr">
         <is>
           <t>Line</t>
         </is>
       </c>
-      <c r="C58" s="3" t="inlineStr">
+      <c r="C58" s="8" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="D58" s="3" t="inlineStr">
+      <c r="D58" s="8" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="E58" s="3" t="inlineStr">
+      <c r="E58" s="8" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
-      <c r="F58" s="4" t="inlineStr">
+      <c r="F58" s="9" t="inlineStr">
         <is>
           <t>Start Time</t>
         </is>
       </c>
-      <c r="G58" s="4" t="inlineStr">
+      <c r="G58" s="9" t="inlineStr">
         <is>
           <t>End Time</t>
         </is>
       </c>
-      <c r="H58" s="4" t="inlineStr">
+      <c r="H58" s="9" t="inlineStr">
         <is>
           <t>UPH</t>
         </is>
       </c>
     </row>
     <row r="59">
-      <c r="B59" s="6" t="n"/>
-      <c r="C59" s="5" t="n"/>
-      <c r="D59" s="5" t="n"/>
-      <c r="E59" s="5" t="n"/>
-      <c r="F59" s="7" t="n"/>
-      <c r="G59" s="7" t="n"/>
-      <c r="H59" s="7" t="n"/>
+      <c r="B59" s="11" t="n"/>
+      <c r="C59" s="10" t="n"/>
+      <c r="D59" s="10" t="n"/>
+      <c r="E59" s="10" t="n"/>
+      <c r="F59" s="12" t="n"/>
+      <c r="G59" s="12" t="n"/>
+      <c r="H59" s="12" t="n"/>
     </row>
     <row r="60">
-      <c r="B60" s="6" t="n"/>
-      <c r="C60" s="5" t="n"/>
-      <c r="D60" s="5" t="n"/>
-      <c r="E60" s="5" t="n"/>
-      <c r="F60" s="7" t="n"/>
-      <c r="G60" s="7" t="n"/>
-      <c r="H60" s="7" t="n"/>
+      <c r="B60" s="11" t="n"/>
+      <c r="C60" s="10" t="n"/>
+      <c r="D60" s="10" t="n"/>
+      <c r="E60" s="10" t="n"/>
+      <c r="F60" s="12" t="n"/>
+      <c r="G60" s="12" t="n"/>
+      <c r="H60" s="12" t="n"/>
     </row>
     <row r="61">
-      <c r="B61" s="6" t="n"/>
-      <c r="C61" s="5" t="n"/>
-      <c r="D61" s="5" t="n"/>
-      <c r="E61" s="5" t="n"/>
-      <c r="F61" s="7" t="n"/>
-      <c r="G61" s="7" t="n"/>
-      <c r="H61" s="7" t="n"/>
+      <c r="B61" s="11" t="n"/>
+      <c r="C61" s="10" t="n"/>
+      <c r="D61" s="10" t="n"/>
+      <c r="E61" s="10" t="n"/>
+      <c r="F61" s="12" t="n"/>
+      <c r="G61" s="12" t="n"/>
+      <c r="H61" s="12" t="n"/>
     </row>
     <row r="62">
-      <c r="B62" s="6" t="n"/>
-      <c r="C62" s="5" t="n"/>
-      <c r="D62" s="5" t="n"/>
-      <c r="E62" s="5" t="n"/>
-      <c r="F62" s="7" t="n"/>
-      <c r="G62" s="7" t="n"/>
-      <c r="H62" s="7" t="n"/>
+      <c r="B62" s="11" t="n"/>
+      <c r="C62" s="10" t="n"/>
+      <c r="D62" s="10" t="n"/>
+      <c r="E62" s="10" t="n"/>
+      <c r="F62" s="12" t="n"/>
+      <c r="G62" s="12" t="n"/>
+      <c r="H62" s="12" t="n"/>
     </row>
     <row r="63">
-      <c r="B63" s="6" t="n"/>
-      <c r="C63" s="5" t="n"/>
-      <c r="D63" s="5" t="n"/>
-      <c r="E63" s="5" t="n"/>
-      <c r="F63" s="7" t="n"/>
-      <c r="G63" s="7" t="n"/>
-      <c r="H63" s="7" t="n"/>
+      <c r="B63" s="11" t="n"/>
+      <c r="C63" s="10" t="n"/>
+      <c r="D63" s="10" t="n"/>
+      <c r="E63" s="10" t="n"/>
+      <c r="F63" s="12" t="n"/>
+      <c r="G63" s="12" t="n"/>
+      <c r="H63" s="12" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="F57:G57"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="F49:G49"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="F32:G32"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:E16"/>
-    <mergeCell ref="F16:G16"/>
+  <mergeCells count="32">
     <mergeCell ref="J7:K7"/>
+    <mergeCell ref="B3:H4"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="E5:G5"/>
     <mergeCell ref="H11:H13"/>
     <mergeCell ref="H18:H19"/>
     <mergeCell ref="H20:H21"/>
@@ -1681,6 +1636,27 @@
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="E20:E21"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:E16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="F32:G32"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="D49:E49"/>
+    <mergeCell ref="F49:G49"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="F57:G57"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
OT table email - EMFP
</commit_message>
<xml_diff>
--- a/Consolidated Factory Workplan.xlsx
+++ b/Consolidated Factory Workplan.xlsx
@@ -16,9 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="[hh]:mm:ss"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <name val="Calibri"/>
@@ -135,7 +133,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -167,7 +165,6 @@
     <xf numFmtId="21" fontId="0" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="3" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
@@ -535,7 +532,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="B3:N63"/>
+  <dimension ref="B3:N66"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -557,16 +554,6 @@
           <t>Updated on :</t>
         </is>
       </c>
-      <c r="F5" s="2" t="inlineStr">
-        <is>
-          <t>12-05-2022 10:44:57</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>+0800</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="B7" s="3" t="inlineStr">
@@ -1035,11 +1022,7 @@
       <c r="K22" s="15" t="n"/>
     </row>
     <row r="23">
-      <c r="B23" s="13" t="inlineStr">
-        <is>
-          <t>ARB</t>
-        </is>
-      </c>
+      <c r="B23" s="13" t="n"/>
       <c r="C23" s="12" t="n"/>
       <c r="D23" s="12" t="n"/>
       <c r="E23" s="12" t="n"/>
@@ -1073,7 +1056,7 @@
       <c r="I24" s="4" t="n"/>
       <c r="J24" s="3" t="inlineStr">
         <is>
-          <t>12-May</t>
+          <t>18-May</t>
         </is>
       </c>
       <c r="K24" s="4" t="n"/>
@@ -1239,11 +1222,7 @@
       <c r="G32" s="5" t="n"/>
       <c r="H32" s="5" t="n"/>
       <c r="I32" s="4" t="n"/>
-      <c r="J32" s="3" t="inlineStr">
-        <is>
-          <t>22-Feb</t>
-        </is>
-      </c>
+      <c r="J32" s="3" t="inlineStr"/>
       <c r="K32" s="4" t="n"/>
     </row>
     <row r="33">
@@ -1304,27 +1283,11 @@
           <t>Desktop</t>
         </is>
       </c>
-      <c r="C34" s="12" t="inlineStr">
-        <is>
-          <t>8am</t>
-        </is>
-      </c>
-      <c r="D34" s="12" t="inlineStr">
-        <is>
-          <t>7pm</t>
-        </is>
-      </c>
+      <c r="C34" s="12" t="n"/>
+      <c r="D34" s="12" t="n"/>
       <c r="E34" s="12" t="n"/>
-      <c r="F34" s="14" t="inlineStr">
-        <is>
-          <t>11am</t>
-        </is>
-      </c>
-      <c r="G34" s="14" t="inlineStr">
-        <is>
-          <t>10pm</t>
-        </is>
-      </c>
+      <c r="F34" s="14" t="n"/>
+      <c r="G34" s="14" t="n"/>
       <c r="H34" s="14" t="n"/>
       <c r="I34" s="15" t="n"/>
       <c r="J34" s="15" t="n"/>
@@ -1336,27 +1299,11 @@
           <t>HYBRID 1</t>
         </is>
       </c>
-      <c r="C35" s="12" t="inlineStr">
-        <is>
-          <t>8am</t>
-        </is>
-      </c>
-      <c r="D35" s="12" t="inlineStr">
-        <is>
-          <t>7pm</t>
-        </is>
-      </c>
+      <c r="C35" s="12" t="n"/>
+      <c r="D35" s="12" t="n"/>
       <c r="E35" s="12" t="n"/>
-      <c r="F35" s="14" t="inlineStr">
-        <is>
-          <t>11am</t>
-        </is>
-      </c>
-      <c r="G35" s="14" t="inlineStr">
-        <is>
-          <t>10pm</t>
-        </is>
-      </c>
+      <c r="F35" s="14" t="n"/>
+      <c r="G35" s="14" t="n"/>
       <c r="H35" s="14" t="n"/>
       <c r="I35" s="15" t="n"/>
       <c r="J35" s="15" t="n"/>
@@ -1368,27 +1315,11 @@
           <t>HYBRID 2</t>
         </is>
       </c>
-      <c r="C36" s="12" t="inlineStr">
-        <is>
-          <t>8am</t>
-        </is>
-      </c>
-      <c r="D36" s="12" t="inlineStr">
-        <is>
-          <t>7pm</t>
-        </is>
-      </c>
+      <c r="C36" s="12" t="n"/>
+      <c r="D36" s="12" t="n"/>
       <c r="E36" s="12" t="n"/>
-      <c r="F36" s="14" t="inlineStr">
-        <is>
-          <t>11am</t>
-        </is>
-      </c>
-      <c r="G36" s="14" t="inlineStr">
-        <is>
-          <t>10pm</t>
-        </is>
-      </c>
+      <c r="F36" s="14" t="n"/>
+      <c r="G36" s="14" t="n"/>
       <c r="H36" s="14" t="n"/>
       <c r="I36" s="15" t="n"/>
       <c r="J36" s="15" t="n"/>
@@ -1400,27 +1331,11 @@
           <t>Server</t>
         </is>
       </c>
-      <c r="C37" s="12" t="inlineStr">
-        <is>
-          <t>8am</t>
-        </is>
-      </c>
-      <c r="D37" s="12" t="inlineStr">
-        <is>
-          <t>7pm</t>
-        </is>
-      </c>
+      <c r="C37" s="12" t="n"/>
+      <c r="D37" s="12" t="n"/>
       <c r="E37" s="12" t="n"/>
-      <c r="F37" s="14" t="inlineStr">
-        <is>
-          <t>11am</t>
-        </is>
-      </c>
-      <c r="G37" s="14" t="inlineStr">
-        <is>
-          <t>10pm</t>
-        </is>
-      </c>
+      <c r="F37" s="14" t="n"/>
+      <c r="G37" s="14" t="n"/>
       <c r="H37" s="14" t="n"/>
       <c r="I37" s="15" t="n"/>
       <c r="J37" s="15" t="n"/>
@@ -1471,11 +1386,7 @@
       <c r="G40" s="5" t="n"/>
       <c r="H40" s="5" t="n"/>
       <c r="I40" s="4" t="n"/>
-      <c r="J40" s="3" t="inlineStr">
-        <is>
-          <t>12-May</t>
-        </is>
-      </c>
+      <c r="J40" s="3" t="inlineStr"/>
       <c r="K40" s="4" t="n"/>
     </row>
     <row r="41">
@@ -1536,27 +1447,11 @@
           <t>Line 1 Frontend</t>
         </is>
       </c>
-      <c r="C42" s="12" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="D42" s="12" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
+      <c r="C42" s="12" t="n"/>
+      <c r="D42" s="12" t="n"/>
       <c r="E42" s="12" t="n"/>
-      <c r="F42" s="14" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="G42" s="14" t="inlineStr">
-        <is>
-          <t>23:45</t>
-        </is>
-      </c>
+      <c r="F42" s="14" t="n"/>
+      <c r="G42" s="14" t="n"/>
       <c r="H42" s="14" t="n"/>
       <c r="I42" s="15" t="n"/>
       <c r="J42" s="15" t="n"/>
@@ -1568,27 +1463,11 @@
           <t>Line 2 Frontend</t>
         </is>
       </c>
-      <c r="C43" s="12" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="D43" s="12" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
+      <c r="C43" s="12" t="n"/>
+      <c r="D43" s="12" t="n"/>
       <c r="E43" s="12" t="n"/>
-      <c r="F43" s="14" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="G43" s="14" t="inlineStr">
-        <is>
-          <t>23:45</t>
-        </is>
-      </c>
+      <c r="F43" s="14" t="n"/>
+      <c r="G43" s="14" t="n"/>
       <c r="H43" s="14" t="n"/>
       <c r="I43" s="15" t="n"/>
       <c r="J43" s="15" t="n"/>
@@ -1600,27 +1479,11 @@
           <t>Line 3 Frontend</t>
         </is>
       </c>
-      <c r="C44" s="12" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="D44" s="12" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
+      <c r="C44" s="12" t="n"/>
+      <c r="D44" s="12" t="n"/>
       <c r="E44" s="12" t="n"/>
-      <c r="F44" s="14" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="G44" s="14" t="inlineStr">
-        <is>
-          <t>23:45</t>
-        </is>
-      </c>
+      <c r="F44" s="14" t="n"/>
+      <c r="G44" s="14" t="n"/>
       <c r="H44" s="14" t="n"/>
       <c r="I44" s="15" t="n"/>
       <c r="J44" s="15" t="n"/>
@@ -1632,16 +1495,8 @@
           <t>Line 1 Backend</t>
         </is>
       </c>
-      <c r="C45" s="12" t="inlineStr">
-        <is>
-          <t>06:00</t>
-        </is>
-      </c>
-      <c r="D45" s="12" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
+      <c r="C45" s="12" t="n"/>
+      <c r="D45" s="12" t="n"/>
       <c r="E45" s="12" t="n"/>
       <c r="F45" s="14" t="n"/>
       <c r="G45" s="14" t="n"/>
@@ -1656,16 +1511,8 @@
           <t>Line 2 Backend</t>
         </is>
       </c>
-      <c r="C46" s="12" t="inlineStr">
-        <is>
-          <t>14:45</t>
-        </is>
-      </c>
-      <c r="D46" s="12" t="inlineStr">
-        <is>
-          <t>23:45</t>
-        </is>
-      </c>
+      <c r="C46" s="12" t="n"/>
+      <c r="D46" s="12" t="n"/>
       <c r="E46" s="12" t="n"/>
       <c r="F46" s="14" t="n"/>
       <c r="G46" s="14" t="n"/>
@@ -1680,8 +1527,8 @@
           <t>Line 3 Backend</t>
         </is>
       </c>
-      <c r="C47" s="12" t="inlineStr"/>
-      <c r="D47" s="12" t="inlineStr"/>
+      <c r="C47" s="12" t="n"/>
+      <c r="D47" s="12" t="n"/>
       <c r="E47" s="12" t="n"/>
       <c r="F47" s="14" t="n"/>
       <c r="G47" s="14" t="n"/>
@@ -1713,7 +1560,7 @@
       <c r="I48" s="4" t="n"/>
       <c r="J48" s="3" t="inlineStr">
         <is>
-          <t>12-May</t>
+          <t>18-May</t>
         </is>
       </c>
       <c r="K48" s="4" t="n"/>
@@ -1776,23 +1623,23 @@
           <t>EMFP</t>
         </is>
       </c>
-      <c r="C50" s="22" t="inlineStr">
+      <c r="C50" s="21" t="inlineStr">
         <is>
           <t>6:00</t>
         </is>
       </c>
-      <c r="D50" s="22" t="inlineStr">
+      <c r="D50" s="21" t="inlineStr">
         <is>
           <t>14:00</t>
         </is>
       </c>
       <c r="E50" s="12" t="n"/>
-      <c r="F50" s="23" t="inlineStr">
+      <c r="F50" s="22" t="inlineStr">
         <is>
           <t>14:00</t>
         </is>
       </c>
-      <c r="G50" s="23" t="inlineStr">
+      <c r="G50" s="22" t="inlineStr">
         <is>
           <t>22:00</t>
         </is>
@@ -1883,11 +1730,7 @@
       <c r="G56" s="5" t="n"/>
       <c r="H56" s="5" t="n"/>
       <c r="I56" s="4" t="n"/>
-      <c r="J56" s="3" t="inlineStr">
-        <is>
-          <t>12-May</t>
-        </is>
-      </c>
+      <c r="J56" s="3" t="inlineStr"/>
       <c r="K56" s="4" t="n"/>
     </row>
     <row r="57">
@@ -1948,29 +1791,12 @@
           <t>Notebook</t>
         </is>
       </c>
-      <c r="C58" s="21" t="inlineStr">
-        <is>
-          <t>8:30:00</t>
-        </is>
-      </c>
-      <c r="D58" s="22">
-        <f>C58 + TIME(7.230000,0,0)</f>
-        <v/>
-      </c>
-      <c r="E58" s="12" t="n">
-        <v>446</v>
-      </c>
-      <c r="F58" s="23">
-        <f>C58 + TIME(7.230000,0,0)</f>
-        <v/>
-      </c>
-      <c r="G58" s="23">
-        <f>F58 + TIME(6.780000,0,0)</f>
-        <v/>
-      </c>
-      <c r="H58" s="14" t="n">
-        <v>394</v>
-      </c>
+      <c r="C58" s="12" t="n"/>
+      <c r="D58" s="12" t="n"/>
+      <c r="E58" s="12" t="n"/>
+      <c r="F58" s="14" t="n"/>
+      <c r="G58" s="14" t="n"/>
+      <c r="H58" s="14" t="n"/>
       <c r="I58" s="15" t="n"/>
       <c r="J58" s="15" t="n"/>
       <c r="K58" s="15" t="n"/>
@@ -1981,29 +1807,12 @@
           <t>Desktop</t>
         </is>
       </c>
-      <c r="C59" s="21" t="inlineStr">
-        <is>
-          <t>8:30:00</t>
-        </is>
-      </c>
-      <c r="D59" s="22">
-        <f>C58 + TIME(7.230000,0,0)</f>
-        <v/>
-      </c>
-      <c r="E59" s="12" t="n">
-        <v>70</v>
-      </c>
-      <c r="F59" s="23">
-        <f>C58 + TIME(7.230000,0,0)</f>
-        <v/>
-      </c>
-      <c r="G59" s="23">
-        <f>F59 + TIME(0.000000,0,0)</f>
-        <v/>
-      </c>
-      <c r="H59" s="14" t="n">
-        <v>0</v>
-      </c>
+      <c r="C59" s="12" t="n"/>
+      <c r="D59" s="12" t="n"/>
+      <c r="E59" s="12" t="n"/>
+      <c r="F59" s="14" t="n"/>
+      <c r="G59" s="14" t="n"/>
+      <c r="H59" s="14" t="n"/>
       <c r="I59" s="15" t="n"/>
       <c r="J59" s="15" t="n"/>
       <c r="K59" s="15" t="n"/>
@@ -2014,29 +1823,12 @@
           <t>Server</t>
         </is>
       </c>
-      <c r="C60" s="21" t="inlineStr">
-        <is>
-          <t>8:30:00</t>
-        </is>
-      </c>
-      <c r="D60" s="22">
-        <f>C58 + TIME(4.000000,0,0)</f>
-        <v/>
-      </c>
-      <c r="E60" s="12" t="n">
-        <v>7.14</v>
-      </c>
-      <c r="F60" s="23">
-        <f>C58 + TIME(4.000000,0,0)</f>
-        <v/>
-      </c>
-      <c r="G60" s="23">
-        <f>F60 + TIME(0.000000,0,0)</f>
-        <v/>
-      </c>
-      <c r="H60" s="14" t="n">
-        <v>0</v>
-      </c>
+      <c r="C60" s="12" t="n"/>
+      <c r="D60" s="12" t="n"/>
+      <c r="E60" s="12" t="n"/>
+      <c r="F60" s="14" t="n"/>
+      <c r="G60" s="14" t="n"/>
+      <c r="H60" s="14" t="n"/>
       <c r="I60" s="15" t="n"/>
       <c r="J60" s="15" t="n"/>
       <c r="K60" s="15" t="n"/>
@@ -2047,29 +1839,12 @@
           <t>AIO</t>
         </is>
       </c>
-      <c r="C61" s="21" t="inlineStr">
-        <is>
-          <t>8:30:00</t>
-        </is>
-      </c>
-      <c r="D61" s="22">
-        <f>C58 + TIME(nan,0,0)</f>
-        <v/>
-      </c>
-      <c r="E61" s="12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F61" s="23">
-        <f>C58 + TIME(nan,0,0)</f>
-        <v/>
-      </c>
-      <c r="G61" s="23">
-        <f>F61 + TIME(nan,0,0)</f>
-        <v/>
-      </c>
-      <c r="H61" s="14" t="n">
-        <v>0</v>
-      </c>
+      <c r="C61" s="12" t="n"/>
+      <c r="D61" s="12" t="n"/>
+      <c r="E61" s="12" t="n"/>
+      <c r="F61" s="14" t="n"/>
+      <c r="G61" s="14" t="n"/>
+      <c r="H61" s="14" t="n"/>
       <c r="I61" s="15" t="n"/>
       <c r="J61" s="15" t="n"/>
       <c r="K61" s="15" t="n"/>
@@ -2097,6 +1872,52 @@
       <c r="I63" s="15" t="n"/>
       <c r="J63" s="15" t="n"/>
       <c r="K63" s="15" t="n"/>
+    </row>
+    <row r="65">
+      <c r="B65" s="6" t="inlineStr">
+        <is>
+          <t>Factory Overtime</t>
+        </is>
+      </c>
+      <c r="C65" s="6" t="inlineStr">
+        <is>
+          <t>E-Mail content</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="B66" s="7" t="inlineStr">
+        <is>
+          <t>EMFP</t>
+        </is>
+      </c>
+      <c r="C66" s="7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dear All,
+Please be informed that on Monday, the 28th of February, EMFP morning shift B will work overtime in the following pattern:
+CSG LOB                  6:05 am -2.05pm
+ISG LOB                   6:00 am -2.00pm
+SHIPPING               6:05 am  -2.05pm     
+Please provide relevant support.
+Please note that overtime may be canceled for unpredicted, important reasons.
+Manager on duty during overtime;
+Regards
+Mariusz Kaczewiak
+EMFP Supervisor, Production Operations
+Mobile: +48 500 216 562
+Dell EMFP Poland
+mariusz.kaczewiak@dell.com &lt;mailto:mariusz.kaczewiak@dell.com&gt; 
+Dell Products (Poland) Sp. z o.o, Łódź, ul. Informatyczna 1
+&amp;
+Maciej Kamiński
+EMFP Manufacturing Operations Supervisor 
+Dell | EMFP Materials
+mobile +48 500 216 519
+maciej_kaminski@dell.com &lt;mailto:maciej_kaminski@dell.com&gt; 
+Dell Products (Poland) Sp. z o.o.,ul. Informatyczna 1
+</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="39">

</xml_diff>